<commit_message>
Api cinema, process in font-end
</commit_message>
<xml_diff>
--- a/design DB.xlsx
+++ b/design DB.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\react-native\MovieApp-ReactNative-Nodejs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6899FA11-FEA1-4712-B79C-F1F148498901}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DD98916-8492-49BC-B204-CF080B50A805}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{83498B1E-B4CB-4C94-8613-9AAE9F2B9CB7}"/>
   </bookViews>
@@ -17,7 +17,6 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1805,7 +1804,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>76420</xdr:colOff>
+      <xdr:colOff>41265</xdr:colOff>
       <xdr:row>12</xdr:row>
       <xdr:rowOff>216935</xdr:rowOff>
     </xdr:to>
@@ -1823,9 +1822,9 @@
       <xdr:grpSpPr>
         <a:xfrm>
           <a:off x="4410075" y="2362200"/>
-          <a:ext cx="809845" cy="712235"/>
+          <a:ext cx="774690" cy="712235"/>
           <a:chOff x="476250" y="228600"/>
-          <a:chExt cx="847945" cy="712235"/>
+          <a:chExt cx="811136" cy="712235"/>
         </a:xfrm>
       </xdr:grpSpPr>
       <xdr:cxnSp macro="">
@@ -1844,8 +1843,8 @@
         </xdr:nvCxnSpPr>
         <xdr:spPr>
           <a:xfrm flipV="1">
-            <a:off x="732410" y="360880"/>
-            <a:ext cx="286765" cy="447675"/>
+            <a:off x="795620" y="360880"/>
+            <a:ext cx="223555" cy="447675"/>
           </a:xfrm>
           <a:prstGeom prst="line">
             <a:avLst/>
@@ -1881,7 +1880,83 @@
         <xdr:spPr>
           <a:xfrm>
             <a:off x="476250" y="676275"/>
-            <a:ext cx="256160" cy="264560"/>
+            <a:ext cx="319370" cy="264560"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+            <a:spAutoFit/>
+          </a:bodyPr>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+              <a:lnSpc>
+                <a:spcPct val="100000"/>
+              </a:lnSpc>
+              <a:spcBef>
+                <a:spcPts val="0"/>
+              </a:spcBef>
+              <a:spcAft>
+                <a:spcPts val="0"/>
+              </a:spcAft>
+              <a:buClrTx/>
+              <a:buSzTx/>
+              <a:buFontTx/>
+              <a:buNone/>
+              <a:tabLst/>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="ja-JP" altLang="ja-JP" sz="1100" b="0" i="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:effectLst/>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:rPr>
+              <a:t>∞</a:t>
+            </a:r>
+            <a:endParaRPr lang="ja-JP" altLang="ja-JP">
+              <a:effectLst/>
+            </a:endParaRPr>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="75" name="TextBox 74">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{37C38D35-0D2A-46F2-BADB-602FE737D070}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="1019175" y="228600"/>
+            <a:ext cx="268211" cy="264560"/>
           </a:xfrm>
           <a:prstGeom prst="rect">
             <a:avLst/>
@@ -1912,64 +1987,6 @@
               <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
               <a:t>1</a:t>
             </a:r>
-            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
-          </a:p>
-        </xdr:txBody>
-      </xdr:sp>
-      <xdr:sp macro="" textlink="">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="75" name="TextBox 74">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{37C38D35-0D2A-46F2-BADB-602FE737D070}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvSpPr txBox="1"/>
-        </xdr:nvSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="1019175" y="228600"/>
-            <a:ext cx="305020" cy="264560"/>
-          </a:xfrm>
-          <a:prstGeom prst="rect">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:noFill/>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="0">
-            <a:scrgbClr r="0" g="0" b="0"/>
-          </a:lnRef>
-          <a:fillRef idx="0">
-            <a:scrgbClr r="0" g="0" b="0"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:scrgbClr r="0" g="0" b="0"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="tx1"/>
-          </a:fontRef>
-        </xdr:style>
-        <xdr:txBody>
-          <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
-            <a:spAutoFit/>
-          </a:bodyPr>
-          <a:lstStyle/>
-          <a:p>
-            <a:r>
-              <a:rPr lang="ja-JP" altLang="en-US" sz="1100" b="0" i="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1"/>
-                </a:solidFill>
-                <a:effectLst/>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:rPr>
-              <a:t>∞</a:t>
-            </a:r>
-            <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
           </a:p>
         </xdr:txBody>
       </xdr:sp>
@@ -2174,7 +2191,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>95470</xdr:colOff>
+      <xdr:colOff>59868</xdr:colOff>
       <xdr:row>17</xdr:row>
       <xdr:rowOff>226460</xdr:rowOff>
     </xdr:to>
@@ -2192,9 +2209,9 @@
       <xdr:grpSpPr>
         <a:xfrm>
           <a:off x="4400550" y="3095625"/>
-          <a:ext cx="838420" cy="1178960"/>
+          <a:ext cx="802818" cy="1178960"/>
           <a:chOff x="476250" y="676275"/>
-          <a:chExt cx="876520" cy="1178960"/>
+          <a:chExt cx="839300" cy="1178960"/>
         </a:xfrm>
       </xdr:grpSpPr>
       <xdr:cxnSp macro="">
@@ -2213,8 +2230,8 @@
         </xdr:nvCxnSpPr>
         <xdr:spPr>
           <a:xfrm>
-            <a:off x="732410" y="808555"/>
-            <a:ext cx="315340" cy="914400"/>
+            <a:off x="795131" y="808555"/>
+            <a:ext cx="252620" cy="914400"/>
           </a:xfrm>
           <a:prstGeom prst="line">
             <a:avLst/>
@@ -2250,7 +2267,83 @@
         <xdr:spPr>
           <a:xfrm>
             <a:off x="476250" y="676275"/>
-            <a:ext cx="256160" cy="264560"/>
+            <a:ext cx="318881" cy="264560"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+            <a:spAutoFit/>
+          </a:bodyPr>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+              <a:lnSpc>
+                <a:spcPct val="100000"/>
+              </a:lnSpc>
+              <a:spcBef>
+                <a:spcPts val="0"/>
+              </a:spcBef>
+              <a:spcAft>
+                <a:spcPts val="0"/>
+              </a:spcAft>
+              <a:buClrTx/>
+              <a:buSzTx/>
+              <a:buFontTx/>
+              <a:buNone/>
+              <a:tabLst/>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="ja-JP" altLang="ja-JP" sz="1100" b="0" i="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:effectLst/>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:rPr>
+              <a:t>∞</a:t>
+            </a:r>
+            <a:endParaRPr lang="ja-JP" altLang="ja-JP">
+              <a:effectLst/>
+            </a:endParaRPr>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="69" name="TextBox 68">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{62D42BAE-35D4-4CE3-A834-E7D6ED0E9264}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="1047750" y="1590675"/>
+            <a:ext cx="267800" cy="264560"/>
           </a:xfrm>
           <a:prstGeom prst="rect">
             <a:avLst/>
@@ -2281,64 +2374,6 @@
               <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
               <a:t>1</a:t>
             </a:r>
-            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
-          </a:p>
-        </xdr:txBody>
-      </xdr:sp>
-      <xdr:sp macro="" textlink="">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="69" name="TextBox 68">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{62D42BAE-35D4-4CE3-A834-E7D6ED0E9264}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvSpPr txBox="1"/>
-        </xdr:nvSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="1047750" y="1590675"/>
-            <a:ext cx="305020" cy="264560"/>
-          </a:xfrm>
-          <a:prstGeom prst="rect">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:noFill/>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="0">
-            <a:scrgbClr r="0" g="0" b="0"/>
-          </a:lnRef>
-          <a:fillRef idx="0">
-            <a:scrgbClr r="0" g="0" b="0"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:scrgbClr r="0" g="0" b="0"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="tx1"/>
-          </a:fontRef>
-        </xdr:style>
-        <xdr:txBody>
-          <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
-            <a:spAutoFit/>
-          </a:bodyPr>
-          <a:lstStyle/>
-          <a:p>
-            <a:r>
-              <a:rPr lang="ja-JP" altLang="en-US" sz="1100" b="0" i="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1"/>
-                </a:solidFill>
-                <a:effectLst/>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:rPr>
-              <a:t>∞</a:t>
-            </a:r>
-            <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
           </a:p>
         </xdr:txBody>
       </xdr:sp>
@@ -2908,13 +2943,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>1123950</xdr:colOff>
+      <xdr:colOff>1133475</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>76420</xdr:colOff>
+      <xdr:colOff>27560</xdr:colOff>
       <xdr:row>4</xdr:row>
       <xdr:rowOff>226460</xdr:rowOff>
     </xdr:to>
@@ -2931,10 +2966,10 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="6267450" y="247650"/>
-          <a:ext cx="828895" cy="931310"/>
-          <a:chOff x="409575" y="-476250"/>
-          <a:chExt cx="828895" cy="931310"/>
+          <a:off x="6276975" y="247650"/>
+          <a:ext cx="770510" cy="931310"/>
+          <a:chOff x="419100" y="-476250"/>
+          <a:chExt cx="770510" cy="931310"/>
         </a:xfrm>
       </xdr:grpSpPr>
       <xdr:cxnSp macro="">
@@ -2953,8 +2988,8 @@
         </xdr:nvCxnSpPr>
         <xdr:spPr>
           <a:xfrm flipV="1">
-            <a:off x="665735" y="-343970"/>
-            <a:ext cx="267715" cy="666750"/>
+            <a:off x="724120" y="-343970"/>
+            <a:ext cx="209330" cy="666750"/>
           </a:xfrm>
           <a:prstGeom prst="line">
             <a:avLst/>
@@ -2989,7 +3024,83 @@
         </xdr:nvSpPr>
         <xdr:spPr>
           <a:xfrm>
-            <a:off x="409575" y="190500"/>
+            <a:off x="419100" y="190500"/>
+            <a:ext cx="305020" cy="264560"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+            <a:spAutoFit/>
+          </a:bodyPr>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+              <a:lnSpc>
+                <a:spcPct val="100000"/>
+              </a:lnSpc>
+              <a:spcBef>
+                <a:spcPts val="0"/>
+              </a:spcBef>
+              <a:spcAft>
+                <a:spcPts val="0"/>
+              </a:spcAft>
+              <a:buClrTx/>
+              <a:buSzTx/>
+              <a:buFontTx/>
+              <a:buNone/>
+              <a:tabLst/>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="ja-JP" altLang="ja-JP" sz="1100" b="0" i="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:effectLst/>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:rPr>
+              <a:t>∞</a:t>
+            </a:r>
+            <a:endParaRPr lang="ja-JP" altLang="ja-JP">
+              <a:effectLst/>
+            </a:endParaRPr>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="89" name="TextBox 88">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5335D767-4D07-4ACB-8F9D-1A5E0055501F}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="933450" y="-476250"/>
             <a:ext cx="256160" cy="264560"/>
           </a:xfrm>
           <a:prstGeom prst="rect">
@@ -3021,64 +3132,6 @@
               <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
               <a:t>1</a:t>
             </a:r>
-            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
-          </a:p>
-        </xdr:txBody>
-      </xdr:sp>
-      <xdr:sp macro="" textlink="">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="89" name="TextBox 88">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5335D767-4D07-4ACB-8F9D-1A5E0055501F}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvSpPr txBox="1"/>
-        </xdr:nvSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="933450" y="-476250"/>
-            <a:ext cx="305020" cy="264560"/>
-          </a:xfrm>
-          <a:prstGeom prst="rect">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:noFill/>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="0">
-            <a:scrgbClr r="0" g="0" b="0"/>
-          </a:lnRef>
-          <a:fillRef idx="0">
-            <a:scrgbClr r="0" g="0" b="0"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:scrgbClr r="0" g="0" b="0"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="tx1"/>
-          </a:fontRef>
-        </xdr:style>
-        <xdr:txBody>
-          <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
-            <a:spAutoFit/>
-          </a:bodyPr>
-          <a:lstStyle/>
-          <a:p>
-            <a:r>
-              <a:rPr lang="ja-JP" altLang="en-US" sz="1100" b="0" i="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1"/>
-                </a:solidFill>
-                <a:effectLst/>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:rPr>
-              <a:t>∞</a:t>
-            </a:r>
-            <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
           </a:p>
         </xdr:txBody>
       </xdr:sp>
@@ -3481,7 +3534,7 @@
   <dimension ref="A1:K33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>

</xml_diff>

<commit_message>
login API, reservation screen
</commit_message>
<xml_diff>
--- a/design DB.xlsx
+++ b/design DB.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\react-native\MovieApp-ReactNative-Nodejs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DD98916-8492-49BC-B204-CF080B50A805}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F12E416-15CD-4BFC-BF4A-2DF91D7696CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{83498B1E-B4CB-4C94-8613-9AAE9F2B9CB7}"/>
+    <workbookView xWindow="29295" yWindow="255" windowWidth="21600" windowHeight="11385" xr2:uid="{83498B1E-B4CB-4C94-8613-9AAE9F2B9CB7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="56">
   <si>
     <t>Cinema</t>
     <phoneticPr fontId="1"/>
@@ -133,10 +133,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>typeName</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>price</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -189,14 +185,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>Cinema-Screen-cal</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>idCinemaCalendar</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>idScreenCalendar</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -249,19 +237,27 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>typeSeatId</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>TypeTicket</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>ticketId</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
     <t>techSub</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>h5</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>h6</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>payment</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>total</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -300,7 +296,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -323,13 +319,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -337,6 +344,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1985,195 +1995,6 @@
           <a:p>
             <a:r>
               <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
-              <a:t>1</a:t>
-            </a:r>
-          </a:p>
-        </xdr:txBody>
-      </xdr:sp>
-    </xdr:grpSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>1133475</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>27560</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>26435</xdr:rowOff>
-    </xdr:to>
-    <xdr:grpSp>
-      <xdr:nvGrpSpPr>
-        <xdr:cNvPr id="50" name="Group 49">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4FC81442-6531-4070-94E0-BA8B192CFB2F}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGrpSpPr/>
-      </xdr:nvGrpSpPr>
-      <xdr:grpSpPr>
-        <a:xfrm>
-          <a:off x="6276975" y="2409825"/>
-          <a:ext cx="770510" cy="712235"/>
-          <a:chOff x="548164" y="228600"/>
-          <a:chExt cx="727171" cy="712235"/>
-        </a:xfrm>
-      </xdr:grpSpPr>
-      <xdr:cxnSp macro="">
-        <xdr:nvCxnSpPr>
-          <xdr:cNvPr id="51" name="Straight Connector 50">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0421CD8A-A842-46D2-A7A8-83B16C1F89EE}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvCxnSpPr>
-            <a:stCxn id="56" idx="3"/>
-            <a:endCxn id="61" idx="1"/>
-          </xdr:cNvCxnSpPr>
-        </xdr:nvCxnSpPr>
-        <xdr:spPr>
-          <a:xfrm flipV="1">
-            <a:off x="836027" y="360880"/>
-            <a:ext cx="183148" cy="447675"/>
-          </a:xfrm>
-          <a:prstGeom prst="line">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:ln w="19050"/>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="1">
-            <a:schemeClr val="dk1"/>
-          </a:lnRef>
-          <a:fillRef idx="0">
-            <a:schemeClr val="dk1"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:schemeClr val="dk1"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="tx1"/>
-          </a:fontRef>
-        </xdr:style>
-      </xdr:cxnSp>
-      <xdr:sp macro="" textlink="">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="56" name="TextBox 55">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E8D655EB-C485-41D8-8766-26C456A577CF}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvSpPr txBox="1"/>
-        </xdr:nvSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="548164" y="676275"/>
-            <a:ext cx="287863" cy="264560"/>
-          </a:xfrm>
-          <a:prstGeom prst="rect">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:noFill/>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="0">
-            <a:scrgbClr r="0" g="0" b="0"/>
-          </a:lnRef>
-          <a:fillRef idx="0">
-            <a:scrgbClr r="0" g="0" b="0"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:scrgbClr r="0" g="0" b="0"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="tx1"/>
-          </a:fontRef>
-        </xdr:style>
-        <xdr:txBody>
-          <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
-            <a:spAutoFit/>
-          </a:bodyPr>
-          <a:lstStyle/>
-          <a:p>
-            <a:r>
-              <a:rPr lang="ja-JP" altLang="ja-JP" sz="1100" b="0" i="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1"/>
-                </a:solidFill>
-                <a:effectLst/>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:rPr>
-              <a:t>∞</a:t>
-            </a:r>
-            <a:endParaRPr lang="ja-JP" altLang="ja-JP">
-              <a:effectLst/>
-            </a:endParaRPr>
-          </a:p>
-        </xdr:txBody>
-      </xdr:sp>
-      <xdr:sp macro="" textlink="">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="61" name="TextBox 60">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{661273EC-FFFE-4D8A-A413-F10231C4D8C5}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvSpPr txBox="1"/>
-        </xdr:nvSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="1019175" y="228600"/>
-            <a:ext cx="256160" cy="264560"/>
-          </a:xfrm>
-          <a:prstGeom prst="rect">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:noFill/>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="0">
-            <a:scrgbClr r="0" g="0" b="0"/>
-          </a:lnRef>
-          <a:fillRef idx="0">
-            <a:scrgbClr r="0" g="0" b="0"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:scrgbClr r="0" g="0" b="0"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="tx1"/>
-          </a:fontRef>
-        </xdr:style>
-        <xdr:txBody>
-          <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
-            <a:spAutoFit/>
-          </a:bodyPr>
-          <a:lstStyle/>
-          <a:p>
-            <a:r>
-              <a:rPr kumimoji="0" lang="en-US" altLang="ja-JP" sz="1100" b="0" i="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1"/>
-                </a:solidFill>
-                <a:effectLst/>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:rPr>
               <a:t>1</a:t>
             </a:r>
           </a:p>
@@ -3531,10 +3352,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C65505F-4586-49C2-891B-A04C7BCE167F}">
-  <dimension ref="A1:K33"/>
+  <dimension ref="A1:L33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H26" sqref="H26"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -3548,7 +3369,7 @@
     <col min="13" max="13" width="17.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -3556,19 +3377,16 @@
         <v>0</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -3584,11 +3402,8 @@
       <c r="I2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="K2" s="2" t="s">
-        <v>1</v>
-      </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -3596,7 +3411,7 @@
         <v>5</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>21</v>
@@ -3604,11 +3419,8 @@
       <c r="I3" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="K3" s="2" t="s">
-        <v>39</v>
-      </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
@@ -3616,63 +3428,66 @@
         <v>6</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>7</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="K4" s="2" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.4">
       <c r="C5" s="2" t="s">
         <v>3</v>
       </c>
       <c r="E5" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="C6" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E6" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="G5" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="I5" s="2" t="s">
-        <v>34</v>
-      </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="C6" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>33</v>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="E7" s="2" t="s">
+        <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="E7" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A10" s="1" t="s">
         <v>19</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="G10" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="I10">
+        <v>1</v>
+      </c>
+      <c r="J10" t="s">
         <v>52</v>
       </c>
-      <c r="I10" s="1" t="s">
-        <v>54</v>
+      <c r="K10">
+        <v>90</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A11" s="2" t="s">
         <v>1</v>
       </c>
@@ -3685,66 +3500,98 @@
       <c r="G11" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="I11" s="2" t="s">
-        <v>1</v>
+      <c r="I11">
+        <v>2</v>
+      </c>
+      <c r="J11" t="s">
+        <v>53</v>
+      </c>
+      <c r="K11">
+        <v>90</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A12" s="2" t="s">
         <v>20</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="I12" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="A13" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="G13" s="2" t="s">
         <v>24</v>
       </c>
+      <c r="I13">
+        <v>1</v>
+      </c>
+      <c r="J13">
+        <v>1</v>
+      </c>
+      <c r="K13">
+        <v>1</v>
+      </c>
+      <c r="L13">
+        <v>1</v>
+      </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A13" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="G13" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="I13" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A14" s="2" t="s">
         <v>22</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="I14" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="G14" s="2" t="s">
         <v>3</v>
       </c>
+      <c r="I14">
+        <v>2</v>
+      </c>
+      <c r="J14">
+        <v>1</v>
+      </c>
+      <c r="K14">
+        <v>2</v>
+      </c>
+      <c r="L14">
+        <v>1</v>
+      </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A15" s="2" t="s">
         <v>23</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="C16" s="3" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.4">
       <c r="G17" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.4">
@@ -3754,12 +3601,12 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.4">
       <c r="G19" s="2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.4">
       <c r="G20" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.4">
@@ -3775,7 +3622,7 @@
         <v>15</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.4">
@@ -3797,7 +3644,7 @@
         <v>16</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.4">
@@ -3808,7 +3655,7 @@
         <v>3</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.4">
@@ -3867,10 +3714,10 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="F1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
save reservation, API, FE
</commit_message>
<xml_diff>
--- a/design DB.xlsx
+++ b/design DB.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\react-native\MovieApp-ReactNative-Nodejs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F12E416-15CD-4BFC-BF4A-2DF91D7696CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B152225B-93C8-4A71-8807-83F89C90AAFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29295" yWindow="255" windowWidth="21600" windowHeight="11385" xr2:uid="{83498B1E-B4CB-4C94-8613-9AAE9F2B9CB7}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{83498B1E-B4CB-4C94-8613-9AAE9F2B9CB7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -3354,8 +3354,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C65505F-4586-49C2-891B-A04C7BCE167F}">
   <dimension ref="A1:L33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O3" sqref="O3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>

</xml_diff>